<commit_message>
src: routes: -user.ts: update so multiple department names can be added for single userId
</commit_message>
<xml_diff>
--- a/templates/user_template.xlsx
+++ b/templates/user_template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://haagahelia-my.sharepoint.com/personal/bgp963_myy_haaga-helia_fi/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\gitRepo\siba-be\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="15" documentId="8_{62035D08-B3B5-4915-9BB8-364475BD9AF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3A3770CF-2D51-40C2-9412-6734F2E67CC6}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2AD3C76-9F83-4B56-9983-6385D3562D62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3510" yWindow="3510" windowWidth="21600" windowHeight="11235" xr2:uid="{62F6EE3A-6D08-43A2-9CB6-016DBF45EA6C}"/>
+    <workbookView xWindow="2295" yWindow="2295" windowWidth="21600" windowHeight="11235" xr2:uid="{62F6EE3A-6D08-43A2-9CB6-016DBF45EA6C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -77,7 +77,7 @@
     <t>add 0 or 1</t>
   </si>
   <si>
-    <t>name of department</t>
+    <t>name of department 1/name of department 2</t>
   </si>
 </sst>
 </file>
@@ -478,7 +478,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
User csv import fixed for commas and space in department names
</commit_message>
<xml_diff>
--- a/templates/user_template.xlsx
+++ b/templates/user_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\gitRepo\siba-be\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_GitRepos\Siba\Siba_be\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88B6E635-F79E-41F3-8015-1D73568BEC14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B4A3239-5C11-4838-B359-F55F9B6A0A52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{62F6EE3A-6D08-43A2-9CB6-016DBF45EA6C}"/>
+    <workbookView xWindow="1860" yWindow="1860" windowWidth="28800" windowHeight="15910" xr2:uid="{62F6EE3A-6D08-43A2-9CB6-016DBF45EA6C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -53,9 +53,6 @@
     <t>isStatist</t>
   </si>
   <si>
-    <t>department</t>
-  </si>
-  <si>
     <t>email-1-@gmail.com</t>
   </si>
   <si>
@@ -78,6 +75,9 @@
   </si>
   <si>
     <t>name of department 1|name of department 2</t>
+  </si>
+  <si>
+    <t>departmentNames</t>
   </si>
 </sst>
 </file>
@@ -478,18 +478,18 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="9.54296875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="19" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -506,67 +506,67 @@
         <v>4</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3" t="s">
         <v>9</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" t="s">
         <v>12</v>
       </c>
-      <c r="D2" t="s">
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" t="s">
         <v>12</v>
-      </c>
-      <c r="E2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F4" t="s">
-        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>